<commit_message>
bodrumi 1 e perfunduar
</commit_message>
<xml_diff>
--- a/5-Njësit-Banesore/regjistri/Regjistri-i-pjeseve-te-nderteses.xlsx
+++ b/5-Njësit-Banesore/regjistri/Regjistri-i-pjeseve-te-nderteses.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ferizaj\Ferizaj\Ingjinierike\mostra-agjension\5.-Njësit-banesore\Regjistri\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kosova\Ferizaj\Ferizaj\Ingjinierike\Unioni-337-0-Objekti\5-Njësit-Banesore\regjistri\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -615,45 +615,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -692,6 +653,45 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1014,7 +1014,7 @@
   <dimension ref="B1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,24 +1036,24 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
     </row>
     <row r="3" spans="2:17" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -1068,18 +1068,18 @@
       <c r="E3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42" t="s">
+      <c r="G3" s="29"/>
+      <c r="H3" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="42"/>
-      <c r="J3" s="46" t="s">
+      <c r="I3" s="29"/>
+      <c r="J3" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="47"/>
+      <c r="K3" s="34"/>
       <c r="L3" s="23" t="s">
         <v>31</v>
       </c>
@@ -1112,18 +1112,18 @@
       <c r="E4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="43">
+      <c r="F4" s="30">
         <v>888.5</v>
       </c>
-      <c r="G4" s="43"/>
-      <c r="H4" s="44" t="s">
+      <c r="G4" s="30"/>
+      <c r="H4" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="44"/>
-      <c r="J4" s="48" t="s">
+      <c r="I4" s="31"/>
+      <c r="J4" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="49"/>
+      <c r="K4" s="36"/>
       <c r="L4" s="21" t="s">
         <v>32</v>
       </c>
@@ -1142,62 +1142,62 @@
       </c>
     </row>
     <row r="5" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
-      <c r="N6" s="38"/>
-      <c r="O6" s="38"/>
-      <c r="P6" s="38"/>
-      <c r="Q6" s="39"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="26"/>
     </row>
     <row r="7" spans="2:17" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="33"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="39"/>
       <c r="F7" s="14" t="s">
         <v>3</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="27" t="s">
+      <c r="H7" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="28"/>
+      <c r="I7" s="47"/>
       <c r="J7" s="14" t="s">
         <v>6</v>
       </c>
@@ -1227,21 +1227,21 @@
       <c r="B8" s="18">
         <v>1</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="36"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="45"/>
       <c r="F8" s="1">
         <v>4</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="29">
+      <c r="H8" s="48">
         <v>8.51</v>
       </c>
-      <c r="I8" s="30"/>
+      <c r="I8" s="49"/>
       <c r="J8" s="1" t="s">
         <v>25</v>
       </c>
@@ -1267,13 +1267,13 @@
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="18"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="36"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="45"/>
       <c r="F9" s="1"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="30"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="49"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -1285,13 +1285,13 @@
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="18"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="36"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="45"/>
       <c r="F10" s="1"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="30"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="49"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -1303,13 +1303,13 @@
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="18"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="26"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="42"/>
       <c r="F11" s="1"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="30"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="49"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1321,13 +1321,13 @@
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="18"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="42"/>
       <c r="F12" s="1"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="30"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="49"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1339,13 +1339,13 @@
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="18"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="26"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="42"/>
       <c r="F13" s="1"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="30"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="49"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -1357,13 +1357,13 @@
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="18"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="26"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="42"/>
       <c r="F14" s="1"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="30"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="49"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1375,13 +1375,13 @@
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="18"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="26"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="42"/>
       <c r="F15" s="1"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="30"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="49"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1393,13 +1393,13 @@
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="18"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="26"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="42"/>
       <c r="F16" s="1"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="30"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="49"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1411,13 +1411,13 @@
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="18"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="26"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="42"/>
       <c r="F17" s="1"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="30"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="49"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1429,13 +1429,13 @@
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="18"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="26"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="42"/>
       <c r="F18" s="1"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="30"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="49"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1447,13 +1447,13 @@
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="18"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="26"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="42"/>
       <c r="F19" s="1"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="30"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="49"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1477,25 +1477,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B6:Q6"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="B5:Q5"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="H7:I7"/>
@@ -1512,6 +1493,25 @@
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="B6:Q6"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B5:Q5"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>